<commit_message>
mise en commentaires des paramètres de recherche qu'on n'utilise plus 0baab6b99789fa53fa82218b2c8e47d9572c41ea
</commit_message>
<xml_diff>
--- a/update-mapping-pn13/ig/CodeSystem-concept-medication-oncofair-codesystem.xlsx
+++ b/update-mapping-pn13/ig/CodeSystem-concept-medication-oncofair-codesystem.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="45">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-06-25T15:16:11+00:00</t>
+    <t>2024-07-01T07:50:29+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>DOMASIA team of the Signal and Image Processing Laboratory (LTSI) and KEREVAL (https://ltsi.univ-rennes.fr)</t>
+  </si>
+  <si>
+    <t>Jurisdiction</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t>Description</t>
@@ -275,7 +281,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -377,66 +383,74 @@
       <c r="A12" t="s" s="2">
         <v>22</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" t="s" s="2">
+        <v>23</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B13" s="2"/>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>24</v>
-      </c>
-      <c r="B14" t="s" s="2">
-        <v>13</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="B14" s="2"/>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>25</v>
-      </c>
-      <c r="B15" s="2"/>
+        <v>26</v>
+      </c>
+      <c r="B15" t="s" s="2">
+        <v>13</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B16" s="2"/>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B17" s="2"/>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B18" s="2"/>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>29</v>
-      </c>
-      <c r="B19" t="s" s="2">
         <v>30</v>
       </c>
+      <c r="B19" s="2"/>
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
         <v>31</v>
       </c>
-      <c r="B20" s="2"/>
+      <c r="B20" t="s" s="2">
+        <v>32</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="B21" t="s" s="2">
         <v>33</v>
+      </c>
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="B22" t="s" s="2">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -454,63 +468,63 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s" s="1">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s" s="1">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s" s="1">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s" s="2">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C5" t="s" s="2">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D5" s="2"/>
     </row>

</xml_diff>